<commit_message>
ships providing dice done, atk-spd-def halfdone
</commit_message>
<xml_diff>
--- a/Ships.xlsx
+++ b/Ships.xlsx
@@ -30,9 +30,6 @@
     <t>ATK</t>
   </si>
   <si>
-    <t>HP</t>
-  </si>
-  <si>
     <t>SPD</t>
   </si>
   <si>
@@ -339,6 +336,9 @@
   </si>
   <si>
     <t>+2 shield</t>
+  </si>
+  <si>
+    <t>DEF</t>
   </si>
 </sst>
 </file>
@@ -824,7 +824,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -846,57 +846,57 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="76.5">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -908,42 +908,42 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>26</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>27</v>
-      </c>
-      <c r="R2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -955,36 +955,36 @@
         <v>6</v>
       </c>
       <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
         <v>32</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" t="s">
         <v>33</v>
       </c>
-      <c r="L3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>34</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>36</v>
-      </c>
-      <c r="R3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -996,33 +996,33 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" t="s">
         <v>41</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>42</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" t="s">
         <v>43</v>
-      </c>
-      <c r="N4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
         <v>45</v>
       </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1034,30 +1034,30 @@
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" t="s">
         <v>47</v>
-      </c>
-      <c r="M5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
         <v>49</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>50</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -1069,33 +1069,33 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" t="s">
         <v>52</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N6" s="2" t="s">
+      <c r="R6" t="s">
         <v>54</v>
-      </c>
-      <c r="R6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1107,30 +1107,30 @@
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1142,36 +1142,36 @@
         <v>5</v>
       </c>
       <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" t="s">
         <v>32</v>
       </c>
-      <c r="H8" t="s">
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" t="s">
         <v>33</v>
       </c>
-      <c r="L8" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>34</v>
       </c>
-      <c r="N8" t="s">
-        <v>35</v>
-      </c>
       <c r="Q8" t="s">
+        <v>58</v>
+      </c>
+      <c r="R8" t="s">
         <v>59</v>
-      </c>
-      <c r="R8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1183,25 +1183,25 @@
         <v>9</v>
       </c>
       <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
         <v>21</v>
       </c>
-      <c r="H9" t="s">
-        <v>22</v>
-      </c>
       <c r="L9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" t="s">
         <v>25</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>26</v>
       </c>
-      <c r="N9" t="s">
-        <v>27</v>
-      </c>
       <c r="O9" t="s">
+        <v>61</v>
+      </c>
+      <c r="R9" t="s">
         <v>62</v>
-      </c>
-      <c r="R9" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1237,197 +1237,197 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" t="s">
         <v>68</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
         <v>69</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" t="s">
         <v>75</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>76</v>
-      </c>
-      <c r="J2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>81</v>
-      </c>
-      <c r="J3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>86</v>
-      </c>
-      <c r="J4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="H5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" t="s">
         <v>89</v>
-      </c>
-      <c r="H5" t="s">
-        <v>81</v>
-      </c>
-      <c r="J5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="H6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" t="s">
         <v>92</v>
-      </c>
-      <c r="H6" t="s">
-        <v>76</v>
-      </c>
-      <c r="J6" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="H7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" t="s">
         <v>97</v>
-      </c>
-      <c r="H7" t="s">
-        <v>81</v>
-      </c>
-      <c r="J7" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>102</v>
-      </c>
-      <c r="J8" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
baked the code in single .rb; ship cards are basically done
</commit_message>
<xml_diff>
--- a/Ships.xlsx
+++ b/Ships.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -339,6 +339,23 @@
   </si>
   <si>
     <t>DEF</t>
+  </si>
+  <si>
+    <t>Proteus</t>
+  </si>
+  <si>
+    <t>(ANY)(SPD)(INT)</t>
+  </si>
+  <si>
+    <t>(LDR)(UTL)(INT)</t>
+  </si>
+  <si>
+    <t>(ATK)(ATK): +1/3 Attack
+(DEF)(DEF): +1/3 Shields</t>
+  </si>
+  <si>
+    <t>Covert Ops.
++1(ATK) when Dictating Range.</t>
   </si>
 </sst>
 </file>
@@ -388,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -396,6 +413,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -821,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1202,6 +1222,38 @@
       </c>
       <c r="R9" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="51">
+      <c r="A10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ships and tactics updated lines, colored icons, prototype ready
</commit_message>
<xml_diff>
--- a/Ships.xlsx
+++ b/Ships.xlsx
@@ -350,12 +350,13 @@
     <t>(LDR)(UTL)(INT)</t>
   </si>
   <si>
-    <t>(ATK)(ATK): +1/3 Attack
-(DEF)(DEF): +1/3 Shields</t>
-  </si>
-  <si>
     <t>Covert Ops.
 +1(ATK) when Dictating Range.</t>
+  </si>
+  <si>
+    <t>(ATK)(ATK): +1/3 Attack
+(DEF)(DEF): +1/3 Shields
+(SPD): +3 Speed, and -2 Shields</t>
   </si>
 </sst>
 </file>
@@ -844,7 +845,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1224,7 +1225,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="51">
+    <row r="10" spans="1:18" ht="89.25">
       <c r="A10" t="s">
         <v>107</v>
       </c>
@@ -1250,10 +1251,10 @@
         <v>109</v>
       </c>
       <c r="I10" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
icons tested, ewar added
</commit_message>
<xml_diff>
--- a/Ships.xlsx
+++ b/Ships.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -83,11 +83,6 @@
     <t>(LDR)(LDR)(LDR)</t>
   </si>
   <si>
-    <t>(DEF)(DEF): +1/3 Shields
-(SPD): +1 Speed
-(LDR): Ignore Skirmish Warfare shields penalty</t>
-  </si>
-  <si>
     <t>Auguror</t>
   </si>
   <si>
@@ -150,11 +145,6 @@
     <t>Legion</t>
   </si>
   <si>
-    <t>(DEF)(DEF): +1/3 Shields
-(SPD): +1 Speed
-(LDR): Ignore Armored Warfare Speed penalty</t>
-  </si>
-  <si>
     <t>Crusader</t>
   </si>
   <si>
@@ -311,6 +301,36 @@
   </si>
   <si>
     <t>Opposing fleet has -1 Attack</t>
+  </si>
+  <si>
+    <t>Blackbird</t>
+  </si>
+  <si>
+    <t>Electronic Warfare Cruiser</t>
+  </si>
+  <si>
+    <t>(ANY)(EWR)</t>
+  </si>
+  <si>
+    <t>(SPD)(EWR)(EWR)</t>
+  </si>
+  <si>
+    <t>ECM Warfare (Before combat with this ship, opponent loses (ATK) from his dice pool)</t>
+  </si>
+  <si>
+    <t>(DEF): +2 Shield
+(SPD): +2 Speed
+(EWR): ECM Warfare (it stacks)</t>
+  </si>
+  <si>
+    <t>(DEF)(DEF): +1/3 Shields
+(SPD): +2 Speed
+(LDR): Ignore Armored Warfare Speed penalty</t>
+  </si>
+  <si>
+    <t>(DEF)(DEF): +1/3 Shields
+(SPD): +2 Speed
+(LDR): Ignore Skirmish Warfare shields penalty</t>
   </si>
 </sst>
 </file>
@@ -357,13 +377,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -789,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -814,7 +837,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -889,22 +912,22 @@
       <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>21</v>
+      <c r="I3" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="J3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="102">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -919,21 +942,21 @@
         <v>19</v>
       </c>
       <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="89.25">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -948,24 +971,24 @@
         <v>12</v>
       </c>
       <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="J5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="76.5">
       <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -980,24 +1003,24 @@
         <v>19</v>
       </c>
       <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" t="s">
         <v>35</v>
-      </c>
-      <c r="J6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="102">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1012,18 +1035,18 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="J7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="102">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -1046,19 +1069,19 @@
       <c r="H8" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>40</v>
+      <c r="I8" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="J8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="76.5">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1079,10 +1102,42 @@
         <v>13</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J9" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="89.25">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1118,197 +1173,197 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>50</v>
-      </c>
-      <c r="I1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="H2" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="J2" t="s">
         <v>57</v>
-      </c>
-      <c r="H2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="F3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="J3" t="s">
         <v>62</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="J4" t="s">
         <v>67</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H4" t="s">
-        <v>68</v>
-      </c>
-      <c r="J4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" t="s">
         <v>70</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" t="s">
-        <v>63</v>
-      </c>
-      <c r="J5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" t="s">
         <v>73</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="H7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" t="s">
         <v>78</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H7" t="s">
-        <v>63</v>
-      </c>
-      <c r="J7" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="G8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="J8" t="s">
         <v>83</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J8" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>